<commit_message>
Added pictures of prices in the BOM
</commit_message>
<xml_diff>
--- a/BOMs/BOM_LCSC.xlsx
+++ b/BOMs/BOM_LCSC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\KiCad\desings\Scorpion max v1-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\KiCad\desings\Scorpion max v1-main\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4FA527-56E1-4790-B554-339290904B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C94137-AB09-4487-A1E5-29638603CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{A023A23C-0FDA-4B2C-91C3-24AB595353E3}"/>
+    <workbookView xWindow="9555" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{A023A23C-0FDA-4B2C-91C3-24AB595353E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="483">
   <si>
     <t>Reference</t>
   </si>
@@ -1482,6 +1482,9 @@
   </si>
   <si>
     <t>Stencil included. 12 boards per panel</t>
+  </si>
+  <si>
+    <t>Price changes a bit here and there with offers so its no 2 days the same</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1494,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="169" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1630,13 +1633,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1651,7 +1654,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1662,35 +1665,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB7B7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFB7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1740,8 +1715,97 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>13608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1612446</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>123034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58CB2B3F-DE21-FA06-AB8F-BD4B1AAD0BAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22492608"/>
+          <a:ext cx="8157482" cy="6395926"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1605642</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>176894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>2864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8493071F-A415-BD13-523A-C8A96ED824AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8149877" y="22465394"/>
+          <a:ext cx="10597564" cy="6493470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2063,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E312B2-2926-4CFE-BA44-A80109AC1CFC}">
   <dimension ref="A1:Y117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G87" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P119" sqref="P119"/>
+    <sheetView tabSelected="1" topLeftCell="B110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,6 +2144,7 @@
     <col min="11" max="12" width="15.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="16" width="12.140625" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" style="2" customWidth="1"/>
@@ -6210,6 +6275,9 @@
         <v>180.74</v>
       </c>
       <c r="P105" s="22"/>
+      <c r="Q105" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B106" s="7">
@@ -6550,6 +6618,7 @@
     <hyperlink ref="K93" r:id="rId177" tooltip="C7434489" display="https://www.lcsc.com/product-detail/C7434489.html" xr:uid="{99B7AACC-AA08-4B8B-BAAF-67AF4599DE77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId178"/>
 </worksheet>
 </file>
 

</xml_diff>